<commit_message>
Corrections done as per review 1
</commit_message>
<xml_diff>
--- a/Project - Stroop Effect.xlsx
+++ b/Project - Stroop Effect.xlsx
@@ -12,33 +12,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+  <si>
+    <t>Congruent x</t>
+  </si>
+  <si>
+    <t>Incongruent y</t>
+  </si>
+  <si>
+    <t>difference y-x</t>
+  </si>
+  <si>
+    <t>diff mean</t>
+  </si>
+  <si>
+    <t>std deviation of differences sd</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Tstat</t>
+  </si>
+  <si>
+    <t>degrees of freedom df</t>
+  </si>
+  <si>
+    <t>Tcritical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample mean of time taken to read congruent list -&gt; </t>
+  </si>
+  <si>
+    <t>----&gt; x_bar</t>
+  </si>
+  <si>
+    <t>Sample mean of time taken to read incongruent list - &gt;</t>
+  </si>
+  <si>
+    <t>----&gt; y-bar</t>
+  </si>
+  <si>
+    <t>Standard deviation of time taken to read congruent list -&gt;</t>
+  </si>
+  <si>
+    <t>Standard deviation of time taken to read incongruent list -&gt;</t>
+  </si>
+  <si>
+    <t>Sample Number</t>
+  </si>
   <si>
     <t>Congruent</t>
   </si>
   <si>
     <t>Incongruent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample mean of time taken to read congruent list -&gt; </t>
-  </si>
-  <si>
-    <t>Sample mean of time taken to read incongruent list - &gt;</t>
-  </si>
-  <si>
-    <t>Standard deviation of time taken to read congruent list -&gt;</t>
-  </si>
-  <si>
-    <t>Standard deviation of time taken to read incongruent list -&gt;</t>
-  </si>
-  <si>
-    <t>Standard Error SE</t>
-  </si>
-  <si>
-    <t>t-statistic</t>
-  </si>
-  <si>
-    <t>Sample Number</t>
   </si>
   <si>
     <t>sample size of  the congruent words list.</t>
@@ -93,11 +120,11 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -224,11 +251,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1432742789"/>
-        <c:axId val="1218030864"/>
+        <c:axId val="617519712"/>
+        <c:axId val="54469245"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1432742789"/>
+        <c:axId val="617519712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -276,10 +303,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1218030864"/>
+        <c:crossAx val="54469245"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1218030864"/>
+        <c:axId val="54469245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +354,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1432742789"/>
+        <c:crossAx val="617519712"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -421,11 +448,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1073166971"/>
-        <c:axId val="422943017"/>
+        <c:axId val="1421237692"/>
+        <c:axId val="1657415969"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1073166971"/>
+        <c:axId val="1421237692"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,10 +484,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="422943017"/>
+        <c:crossAx val="1657415969"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422943017"/>
+        <c:axId val="1657415969"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +535,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1073166971"/>
+        <c:crossAx val="1421237692"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -597,48 +624,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>12.079</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>19.278</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2.0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>16.791</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>18.741</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>3.0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>9.564</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>21.214</v>
       </c>
       <c r="E4">
@@ -647,38 +674,38 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>4.0</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>8.63</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>15.687</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>5.0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>14.669</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>22.803</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>6.0</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>12.238</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>20.878</v>
       </c>
       <c r="E7">
@@ -687,38 +714,38 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>7.0</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>14.692</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>24.572</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>8.0</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>8.987</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>17.394</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>9.0</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>9.401</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>20.762</v>
       </c>
       <c r="E10">
@@ -727,38 +754,38 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>10.0</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>14.48</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>26.282</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>11.0</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>22.328</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>24.524</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>5</v>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>12.0</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>15.298</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>18.644</v>
       </c>
       <c r="E13">
@@ -767,38 +794,38 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>13.0</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>15.073</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>17.51</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>14.0</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>16.929</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>20.33</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>15.0</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>18.2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>35.255</v>
       </c>
       <c r="E16">
@@ -807,38 +834,38 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>16.0</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>12.13</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>22.158</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>17.0</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>18.495</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>25.139</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>18.0</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>10.639</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>20.429</v>
       </c>
       <c r="E19">
@@ -847,68 +874,68 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>19.0</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>11.344</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>17.425</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>20.0</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>12.369</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>34.288</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>21.0</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>12.944</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>23.894</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>22.0</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="3">
         <v>14.233</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>17.96</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>23.0</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>19.71</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>22.058</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>24.0</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>16.004</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>21.157</v>
       </c>
     </row>
@@ -936,248 +963,405 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>12.079</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>19.278</v>
       </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C25" si="1">B2-A2</f>
+        <v>7.199</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>16.791</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>18.741</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
+      <c r="C3">
+        <f t="shared" si="1"/>
+        <v>1.95</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>9.564</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>21.214</v>
       </c>
-      <c r="D4">
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>8.63</v>
+      </c>
+      <c r="B5" s="3">
+        <v>15.687</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>7.057</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>14.669</v>
+      </c>
+      <c r="B6" s="3">
+        <v>22.803</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>8.134</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(C2-C25)</f>
+        <v>2.046</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>12.238</v>
+      </c>
+      <c r="B7" s="3">
+        <v>20.878</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>14.692</v>
+      </c>
+      <c r="B8" s="3">
+        <v>24.572</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>9.88</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>8.987</v>
+      </c>
+      <c r="B9" s="3">
+        <v>17.394</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>8.407</v>
+      </c>
+      <c r="E9">
+        <f>STDEV(C2:C25)</f>
+        <v>4.86482691</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>9.401</v>
+      </c>
+      <c r="B10" s="3">
+        <v>20.762</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>11.361</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>14.48</v>
+      </c>
+      <c r="B11" s="3">
+        <v>26.282</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>11.802</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>22.328</v>
+      </c>
+      <c r="B12" s="3">
+        <v>24.524</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>2.196</v>
+      </c>
+      <c r="E12">
+        <f>$E$9/sqrt(24)</f>
+        <v>0.9930286348</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>15.298</v>
+      </c>
+      <c r="B13" s="3">
+        <v>18.644</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>3.346</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>15.073</v>
+      </c>
+      <c r="B14" s="3">
+        <v>17.51</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2.437</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>16.929</v>
+      </c>
+      <c r="B15" s="3">
+        <v>20.33</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>3.401</v>
+      </c>
+      <c r="E15">
+        <f>$E$6/$E$12</f>
+        <v>2.060363547</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>18.2</v>
+      </c>
+      <c r="B16" s="3">
+        <v>35.255</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>17.055</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>12.13</v>
+      </c>
+      <c r="B17" s="3">
+        <v>22.158</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>10.028</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3">
+        <v>18.495</v>
+      </c>
+      <c r="B18" s="3">
+        <v>25.139</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>6.644</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
+        <v>10.639</v>
+      </c>
+      <c r="B19" s="3">
+        <v>20.429</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>9.79</v>
+      </c>
+      <c r="E19">
+        <f>24-1</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <v>11.344</v>
+      </c>
+      <c r="B20" s="3">
+        <v>17.425</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>6.081</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>12.369</v>
+      </c>
+      <c r="B21" s="3">
+        <v>34.288</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>21.919</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>12.944</v>
+      </c>
+      <c r="B22" s="3">
+        <v>23.894</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>10.95</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.714</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>14.233</v>
+      </c>
+      <c r="B23" s="3">
+        <v>17.96</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>3.727</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>19.71</v>
+      </c>
+      <c r="B24" s="3">
+        <v>22.058</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2.348</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>16.004</v>
+      </c>
+      <c r="B25" s="3">
+        <v>21.157</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>5.153</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
         <f>average(A2:A25)</f>
         <v>14.051125</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>8.63</v>
-      </c>
-      <c r="B5" s="2">
-        <v>15.687</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>14.669</v>
-      </c>
-      <c r="B6" s="2">
-        <v>22.803</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>12.238</v>
-      </c>
-      <c r="B7" s="2">
-        <v>20.878</v>
-      </c>
-      <c r="D7">
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
         <f>AVERAGE(B2:B25)</f>
         <v>22.01591667</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>14.692</v>
-      </c>
-      <c r="B8" s="2">
-        <v>24.572</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>8.987</v>
-      </c>
-      <c r="B9" s="2">
-        <v>17.394</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <v>9.401</v>
-      </c>
-      <c r="B10" s="2">
-        <v>20.762</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4">
         <f>stdev(A2:A25)</f>
         <v>3.559357958</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <v>14.48</v>
-      </c>
-      <c r="B11" s="2">
-        <v>26.282</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
-        <v>22.328</v>
-      </c>
-      <c r="B12" s="2">
-        <v>24.524</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2">
-        <v>15.298</v>
-      </c>
-      <c r="B13" s="2">
-        <v>18.644</v>
-      </c>
-      <c r="D13">
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
         <f>stdev(B2:B25)</f>
         <v>4.797057122</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2">
-        <v>15.073</v>
-      </c>
-      <c r="B14" s="2">
-        <v>17.51</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2">
-        <v>16.929</v>
-      </c>
-      <c r="B15" s="2">
-        <v>20.33</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2">
-        <v>18.2</v>
-      </c>
-      <c r="B16" s="2">
-        <v>35.255</v>
-      </c>
-      <c r="D16">
-        <f>sqrt(($D$10^2 + $D$13^2)/24)</f>
-        <v>1.219302842</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2">
-        <v>12.13</v>
-      </c>
-      <c r="B17" s="2">
-        <v>22.158</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2">
-        <v>18.495</v>
-      </c>
-      <c r="B18" s="2">
-        <v>25.139</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2">
-        <v>10.639</v>
-      </c>
-      <c r="B19" s="2">
-        <v>20.429</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2">
-        <v>11.344</v>
-      </c>
-      <c r="B20" s="2">
-        <v>17.425</v>
-      </c>
-      <c r="D20">
-        <f>($D$7 - $D$4)/$D$16</f>
-        <v>6.532250554</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2">
-        <v>12.369</v>
-      </c>
-      <c r="B21" s="2">
-        <v>34.288</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2">
-        <v>12.944</v>
-      </c>
-      <c r="B22" s="2">
-        <v>23.894</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2">
-        <v>14.233</v>
-      </c>
-      <c r="B23" s="2">
-        <v>17.96</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="2">
-        <v>19.71</v>
-      </c>
-      <c r="B24" s="2">
-        <v>22.058</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2">
-        <v>16.004</v>
-      </c>
-      <c r="B25" s="2">
-        <v>21.157</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
+    <row r="44">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Corrections made for review 3
</commit_message>
<xml_diff>
--- a/Project - Stroop Effect.xlsx
+++ b/Project - Stroop Effect.xlsx
@@ -38,7 +38,7 @@
     <t>degrees of freedom df</t>
   </si>
   <si>
-    <t>Tcritical</t>
+    <t>Tcritical (2-tailed)</t>
   </si>
   <si>
     <t xml:space="preserve">Sample mean of time taken to read congruent list -&gt; </t>
@@ -251,11 +251,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="617519712"/>
-        <c:axId val="54469245"/>
+        <c:axId val="154405040"/>
+        <c:axId val="1510337285"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="617519712"/>
+        <c:axId val="154405040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,10 +303,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54469245"/>
+        <c:crossAx val="1510337285"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54469245"/>
+        <c:axId val="1510337285"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +354,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617519712"/>
+        <c:crossAx val="154405040"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -448,11 +448,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1421237692"/>
-        <c:axId val="1657415969"/>
+        <c:axId val="1754893182"/>
+        <c:axId val="1377514576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1421237692"/>
+        <c:axId val="1754893182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,10 +484,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1657415969"/>
+        <c:crossAx val="1377514576"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1657415969"/>
+        <c:axId val="1377514576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +535,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1421237692"/>
+        <c:crossAx val="1754893182"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -975,8 +975,8 @@
         <v>19.278</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C25" si="1">B2-A2</f>
-        <v>7.199</v>
+        <f>A2-B2</f>
+        <v>-7.199</v>
       </c>
     </row>
     <row r="3">
@@ -987,7 +987,7 @@
         <v>18.741</v>
       </c>
       <c r="C3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C3:C25" si="1">B3-A3</f>
         <v>1.95</v>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="E6">
         <f>AVERAGE(C2-C25)</f>
-        <v>2.046</v>
+        <v>-12.352</v>
       </c>
     </row>
     <row r="7">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E9">
         <f>STDEV(C2:C25)</f>
-        <v>4.86482691</v>
+        <v>5.767400818</v>
       </c>
     </row>
     <row r="10">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E12">
         <f>$E$9/sqrt(24)</f>
-        <v>0.9930286348</v>
+        <v>1.177265762</v>
       </c>
     </row>
     <row r="13">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E15">
         <f>$E$6/$E$12</f>
-        <v>2.060363547</v>
+        <v>-10.49210841</v>
       </c>
     </row>
     <row r="16">
@@ -1257,7 +1257,7 @@
         <v>10.95</v>
       </c>
       <c r="E22" s="2">
-        <v>1.714</v>
+        <v>2.069</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
Changes done as per revie
</commit_message>
<xml_diff>
--- a/Project - Stroop Effect.xlsx
+++ b/Project - Stroop Effect.xlsx
@@ -23,22 +23,22 @@
     <t>difference y-x</t>
   </si>
   <si>
-    <t>diff mean</t>
-  </si>
-  <si>
-    <t>std deviation of differences sd</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>Tstat</t>
-  </si>
-  <si>
-    <t>degrees of freedom df</t>
-  </si>
-  <si>
-    <t>Tcritical (2-tailed)</t>
+    <t>(diff-diff_mean)^2</t>
+  </si>
+  <si>
+    <t>diff_mean</t>
+  </si>
+  <si>
+    <t>sum of dev</t>
+  </si>
+  <si>
+    <t>Squared dev diff  S</t>
+  </si>
+  <si>
+    <t>S/sqrt(n)</t>
+  </si>
+  <si>
+    <t>t_stat</t>
   </si>
   <si>
     <t xml:space="preserve">Sample mean of time taken to read congruent list -&gt; </t>
@@ -251,11 +251,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="154405040"/>
-        <c:axId val="1510337285"/>
+        <c:axId val="944057647"/>
+        <c:axId val="359653563"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154405040"/>
+        <c:axId val="944057647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,10 +303,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1510337285"/>
+        <c:crossAx val="359653563"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1510337285"/>
+        <c:axId val="359653563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +354,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154405040"/>
+        <c:crossAx val="944057647"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -448,11 +448,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1754893182"/>
-        <c:axId val="1377514576"/>
+        <c:axId val="423088838"/>
+        <c:axId val="954244376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1754893182"/>
+        <c:axId val="423088838"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,10 +484,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1377514576"/>
+        <c:crossAx val="954244376"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1377514576"/>
+        <c:axId val="954244376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +535,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1754893182"/>
+        <c:crossAx val="423088838"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -966,6 +966,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3">
@@ -975,8 +978,12 @@
         <v>19.278</v>
       </c>
       <c r="C2">
-        <f>A2-B2</f>
+        <f t="shared" ref="C2:C25" si="1">A2-B2</f>
         <v>-7.199</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D25" si="2">(C2-$G$4)^2</f>
+        <v>0.5864368767</v>
       </c>
     </row>
     <row r="3">
@@ -987,8 +994,15 @@
         <v>18.741</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C25" si="1">B3-A3</f>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>-1.95</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="2"/>
+        <v>36.17771879</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -1000,7 +1014,15 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>11.65</v>
+        <v>-11.65</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>13.58076046</v>
+      </c>
+      <c r="G4">
+        <f>average(C2:C25)</f>
+        <v>-7.964791667</v>
       </c>
     </row>
     <row r="5">
@@ -1012,11 +1034,13 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>7.057</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>-7.057</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>0.8240857101</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -1027,11 +1051,11 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>8.134</v>
-      </c>
-      <c r="E6">
-        <f>AVERAGE(C2-C25)</f>
-        <v>-12.352</v>
+        <v>-8.134</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.02863146007</v>
       </c>
     </row>
     <row r="7">
@@ -1043,7 +1067,14 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>8.64</v>
+        <v>-8.64</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.4559062934</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -1055,10 +1086,15 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>9.88</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
+        <v>-9.88</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>3.66802296</v>
+      </c>
+      <c r="G8" s="2">
+        <f>sum(D2:D25)</f>
+        <v>544.33044</v>
       </c>
     </row>
     <row r="9">
@@ -1070,11 +1106,11 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>8.407</v>
-      </c>
-      <c r="E9">
-        <f>STDEV(C2:C25)</f>
-        <v>5.767400818</v>
+        <v>-8.407</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.1955482101</v>
       </c>
     </row>
     <row r="10">
@@ -1086,7 +1122,11 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>11.361</v>
+        <v>-11.361</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>11.53423104</v>
       </c>
     </row>
     <row r="11">
@@ -1098,10 +1138,14 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>11.802</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>-11.802</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>14.72416779</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -1113,11 +1157,15 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>2.196</v>
-      </c>
-      <c r="E12">
-        <f>$E$9/sqrt(24)</f>
-        <v>1.177265762</v>
+        <v>-2.196</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>33.27895729</v>
+      </c>
+      <c r="G12">
+        <f>sqrt($G$8/24)</f>
+        <v>4.76239803</v>
       </c>
     </row>
     <row r="13">
@@ -1129,7 +1177,11 @@
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>3.346</v>
+        <v>-3.346</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>21.33323646</v>
       </c>
     </row>
     <row r="14">
@@ -1141,10 +1193,14 @@
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>2.437</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
+        <v>-2.437</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>30.55648071</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -1156,11 +1212,15 @@
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>3.401</v>
-      </c>
-      <c r="E15">
-        <f>$E$6/$E$12</f>
-        <v>-10.49210841</v>
+        <v>-3.401</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>20.82819438</v>
+      </c>
+      <c r="G15">
+        <f>$G$12/sqrt(24)</f>
+        <v>0.9721204272</v>
       </c>
     </row>
     <row r="16">
@@ -1172,7 +1232,11 @@
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>17.055</v>
+        <v>-17.055</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>82.63188754</v>
       </c>
     </row>
     <row r="17">
@@ -1184,7 +1248,14 @@
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>10.028</v>
+        <v>-10.028</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>4.256828627</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -1196,10 +1267,15 @@
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>6.644</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>7</v>
+        <v>-6.644</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>1.744490627</v>
+      </c>
+      <c r="G18">
+        <f>($A$30 - $A$33)/($G$15)</f>
+        <v>-8.193215001</v>
       </c>
     </row>
     <row r="19">
@@ -1211,11 +1287,11 @@
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>9.79</v>
-      </c>
-      <c r="E19">
-        <f>24-1</f>
-        <v>23</v>
+        <v>-9.79</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>3.33138546</v>
       </c>
     </row>
     <row r="20">
@@ -1227,8 +1303,13 @@
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>6.081</v>
-      </c>
+        <v>-6.081</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>3.548671043</v>
+      </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="3">
@@ -1239,10 +1320,11 @@
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>21.919</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>8</v>
+        <v>-21.919</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>194.7199302</v>
       </c>
     </row>
     <row r="22">
@@ -1254,10 +1336,11 @@
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>10.95</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2.069</v>
+        <v>-10.95</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>8.911468793</v>
       </c>
     </row>
     <row r="23">
@@ -1269,9 +1352,13 @@
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>3.727</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>-3.727</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>17.95887821</v>
+      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="3">
@@ -1282,7 +1369,11 @@
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>2.348</v>
+        <v>-2.348</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>31.54834863</v>
       </c>
     </row>
     <row r="25">
@@ -1294,12 +1385,19 @@
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>5.153</v>
+        <v>-5.153</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>7.906172377</v>
       </c>
     </row>
     <row r="26">
       <c r="D26" s="2"/>
       <c r="F26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="G27" s="2"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
@@ -1314,6 +1412,10 @@
       <c r="B30" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="G31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">

</xml_diff>